<commit_message>
correção nos dados e inicio da analise PNAD 2009
</commit_message>
<xml_diff>
--- a/analises_vitimizacao/dados_tratados/PNAD_2009/xlsx/agressao/cv126011a.xlsx
+++ b/analises_vitimizacao/dados_tratados/PNAD_2009/xlsx/agressao/cv126011a.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>total(1)</t>
   </si>
@@ -25,7 +25,7 @@
     <t>cor ou raça</t>
   </si>
   <si>
-    <t>unnamed: 1_level_1</t>
+    <t>total</t>
   </si>
   <si>
     <t>homens</t>
@@ -43,16 +43,10 @@
     <t xml:space="preserve">               brasil</t>
   </si>
   <si>
-    <t>situação do domicílio</t>
-  </si>
-  <si>
     <t>urbana</t>
   </si>
   <si>
     <t>rural</t>
-  </si>
-  <si>
-    <t>grandes regiões e unidades da federação</t>
   </si>
   <si>
     <t>norte</t>
@@ -506,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,25 +562,40 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B5">
+        <v>2.33</v>
+      </c>
+      <c r="C5">
+        <v>2.68</v>
+      </c>
+      <c r="D5">
+        <v>2.91</v>
+      </c>
+      <c r="E5">
+        <v>3.09</v>
+      </c>
+      <c r="F5">
+        <v>2.86</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>2.33</v>
+        <v>7.28</v>
       </c>
       <c r="C6">
-        <v>2.68</v>
+        <v>8.16</v>
       </c>
       <c r="D6">
-        <v>2.91</v>
+        <v>9.43</v>
       </c>
       <c r="E6">
-        <v>3.09</v>
+        <v>10.66</v>
       </c>
       <c r="F6">
-        <v>2.86</v>
+        <v>8.109999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -594,44 +603,59 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>7.28</v>
+        <v>5.08</v>
       </c>
       <c r="C7">
-        <v>8.16</v>
+        <v>5.47</v>
       </c>
       <c r="D7">
-        <v>9.43</v>
+        <v>7.34</v>
       </c>
       <c r="E7">
-        <v>10.66</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="F7">
-        <v>8.109999999999999</v>
+        <v>5.19</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B8">
+        <v>15.48</v>
+      </c>
+      <c r="C8">
+        <v>21.57</v>
+      </c>
+      <c r="D8">
+        <v>12.42</v>
+      </c>
+      <c r="E8">
+        <v>21.66</v>
+      </c>
+      <c r="F8">
+        <v>15.79</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>5.08</v>
+        <v>21.99</v>
       </c>
       <c r="C9">
-        <v>5.47</v>
+        <v>20.6</v>
       </c>
       <c r="D9">
-        <v>7.34</v>
+        <v>26.85</v>
       </c>
       <c r="E9">
-        <v>9.220000000000001</v>
+        <v>44.59</v>
       </c>
       <c r="F9">
-        <v>5.19</v>
+        <v>15.11</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -639,19 +663,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>15.48</v>
+        <v>12.95</v>
       </c>
       <c r="C10">
-        <v>21.57</v>
+        <v>12.82</v>
       </c>
       <c r="D10">
-        <v>12.42</v>
+        <v>21.71</v>
       </c>
       <c r="E10">
-        <v>21.66</v>
+        <v>27.6</v>
       </c>
       <c r="F10">
-        <v>15.79</v>
+        <v>14.52</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -659,19 +683,19 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>21.99</v>
+        <v>16.55</v>
       </c>
       <c r="C11">
-        <v>20.6</v>
+        <v>24.38</v>
       </c>
       <c r="D11">
-        <v>26.85</v>
+        <v>24.4</v>
       </c>
       <c r="E11">
-        <v>44.59</v>
+        <v>23.16</v>
       </c>
       <c r="F11">
-        <v>15.11</v>
+        <v>22.53</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -679,19 +703,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>12.95</v>
+        <v>7.58</v>
       </c>
       <c r="C12">
-        <v>12.82</v>
+        <v>7.9</v>
       </c>
       <c r="D12">
-        <v>21.71</v>
+        <v>11.18</v>
       </c>
       <c r="E12">
-        <v>27.6</v>
+        <v>15.12</v>
       </c>
       <c r="F12">
-        <v>14.52</v>
+        <v>7.49</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -699,19 +723,19 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>16.55</v>
+        <v>18.56</v>
       </c>
       <c r="C13">
-        <v>24.38</v>
+        <v>20.32</v>
       </c>
       <c r="D13">
-        <v>24.4</v>
+        <v>27.95</v>
       </c>
       <c r="E13">
-        <v>23.16</v>
+        <v>25.25</v>
       </c>
       <c r="F13">
-        <v>22.53</v>
+        <v>19.16</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -719,19 +743,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>7.58</v>
+        <v>14.34</v>
       </c>
       <c r="C14">
-        <v>7.9</v>
+        <v>14.68</v>
       </c>
       <c r="D14">
-        <v>11.18</v>
+        <v>24.46</v>
       </c>
       <c r="E14">
-        <v>15.12</v>
+        <v>23.81</v>
       </c>
       <c r="F14">
-        <v>7.49</v>
+        <v>17.1</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -739,19 +763,19 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>18.56</v>
+        <v>4.1</v>
       </c>
       <c r="C15">
-        <v>20.32</v>
+        <v>4.76</v>
       </c>
       <c r="D15">
-        <v>27.95</v>
+        <v>4.94</v>
       </c>
       <c r="E15">
-        <v>25.25</v>
+        <v>6.15</v>
       </c>
       <c r="F15">
-        <v>19.16</v>
+        <v>4.47</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -759,19 +783,19 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>14.34</v>
+        <v>17.52</v>
       </c>
       <c r="C16">
-        <v>14.68</v>
+        <v>20.98</v>
       </c>
       <c r="D16">
-        <v>24.46</v>
+        <v>17</v>
       </c>
       <c r="E16">
-        <v>23.81</v>
+        <v>16.35</v>
       </c>
       <c r="F16">
-        <v>17.1</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -779,19 +803,19 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>4.1</v>
+        <v>15.4</v>
       </c>
       <c r="C17">
-        <v>4.76</v>
+        <v>16.45</v>
       </c>
       <c r="D17">
-        <v>4.94</v>
+        <v>18.24</v>
       </c>
       <c r="E17">
-        <v>6.15</v>
+        <v>30</v>
       </c>
       <c r="F17">
-        <v>4.47</v>
+        <v>14.74</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -799,19 +823,19 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>17.52</v>
+        <v>8.67</v>
       </c>
       <c r="C18">
-        <v>20.98</v>
+        <v>8.19</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>13.53</v>
       </c>
       <c r="E18">
-        <v>16.35</v>
+        <v>14.51</v>
       </c>
       <c r="F18">
-        <v>20.9</v>
+        <v>8.98</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -819,19 +843,19 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>15.4</v>
+        <v>14.77</v>
       </c>
       <c r="C19">
-        <v>16.45</v>
+        <v>15.56</v>
       </c>
       <c r="D19">
-        <v>18.24</v>
+        <v>17.49</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>18.66</v>
       </c>
       <c r="F19">
-        <v>14.74</v>
+        <v>16.11</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -839,19 +863,19 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>8.67</v>
+        <v>18.73</v>
       </c>
       <c r="C20">
-        <v>8.19</v>
+        <v>17.79</v>
       </c>
       <c r="D20">
-        <v>13.53</v>
+        <v>25.36</v>
       </c>
       <c r="E20">
-        <v>14.51</v>
+        <v>21.88</v>
       </c>
       <c r="F20">
-        <v>8.98</v>
+        <v>19.89</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -859,19 +883,19 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>14.77</v>
+        <v>6.58</v>
       </c>
       <c r="C21">
-        <v>15.56</v>
+        <v>7.96</v>
       </c>
       <c r="D21">
-        <v>17.49</v>
+        <v>9.18</v>
       </c>
       <c r="E21">
-        <v>18.66</v>
+        <v>11.82</v>
       </c>
       <c r="F21">
-        <v>16.11</v>
+        <v>7.91</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -879,19 +903,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>18.73</v>
+        <v>13.05</v>
       </c>
       <c r="C22">
-        <v>17.79</v>
+        <v>12.71</v>
       </c>
       <c r="D22">
-        <v>25.36</v>
+        <v>21.53</v>
       </c>
       <c r="E22">
-        <v>21.88</v>
+        <v>38.43</v>
       </c>
       <c r="F22">
-        <v>19.89</v>
+        <v>14.52</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -899,19 +923,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>6.58</v>
+        <v>20.21</v>
       </c>
       <c r="C23">
-        <v>7.96</v>
+        <v>23.62</v>
       </c>
       <c r="D23">
-        <v>9.18</v>
+        <v>20.23</v>
       </c>
       <c r="E23">
-        <v>11.82</v>
+        <v>31.83</v>
       </c>
       <c r="F23">
-        <v>7.91</v>
+        <v>22.86</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -919,19 +943,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>13.05</v>
+        <v>6.1</v>
       </c>
       <c r="C24">
-        <v>12.71</v>
+        <v>7.01</v>
       </c>
       <c r="D24">
-        <v>21.53</v>
+        <v>8.32</v>
       </c>
       <c r="E24">
-        <v>38.43</v>
+        <v>15.22</v>
       </c>
       <c r="F24">
-        <v>14.52</v>
+        <v>5.97</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -939,19 +963,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>20.21</v>
+        <v>3.93</v>
       </c>
       <c r="C25">
-        <v>23.62</v>
+        <v>4.68</v>
       </c>
       <c r="D25">
-        <v>20.23</v>
+        <v>4.89</v>
       </c>
       <c r="E25">
-        <v>31.83</v>
+        <v>4.89</v>
       </c>
       <c r="F25">
-        <v>22.86</v>
+        <v>5.17</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -959,19 +983,19 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>6.1</v>
+        <v>7.32</v>
       </c>
       <c r="C26">
-        <v>7.01</v>
+        <v>8.49</v>
       </c>
       <c r="D26">
-        <v>8.32</v>
+        <v>8.57</v>
       </c>
       <c r="E26">
-        <v>15.22</v>
+        <v>11.86</v>
       </c>
       <c r="F26">
-        <v>5.97</v>
+        <v>7.64</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -979,19 +1003,19 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>3.93</v>
+        <v>13.89</v>
       </c>
       <c r="C27">
-        <v>4.68</v>
+        <v>19.09</v>
       </c>
       <c r="D27">
-        <v>4.89</v>
+        <v>18.66</v>
       </c>
       <c r="E27">
-        <v>4.89</v>
+        <v>16.87</v>
       </c>
       <c r="F27">
-        <v>5.17</v>
+        <v>16.69</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -999,19 +1023,19 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>7.32</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="C28">
-        <v>8.49</v>
+        <v>10.49</v>
       </c>
       <c r="D28">
-        <v>8.57</v>
+        <v>10.6</v>
       </c>
       <c r="E28">
-        <v>11.86</v>
+        <v>10.5</v>
       </c>
       <c r="F28">
-        <v>7.64</v>
+        <v>11.21</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1019,19 +1043,19 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>13.89</v>
+        <v>5.81</v>
       </c>
       <c r="C29">
-        <v>19.09</v>
+        <v>6.81</v>
       </c>
       <c r="D29">
-        <v>18.66</v>
+        <v>7.45</v>
       </c>
       <c r="E29">
-        <v>16.87</v>
+        <v>6.41</v>
       </c>
       <c r="F29">
-        <v>16.69</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1039,19 +1063,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>8.289999999999999</v>
+        <v>4.82</v>
       </c>
       <c r="C30">
-        <v>10.49</v>
+        <v>5.28</v>
       </c>
       <c r="D30">
-        <v>10.6</v>
+        <v>6.36</v>
       </c>
       <c r="E30">
-        <v>10.5</v>
+        <v>5.33</v>
       </c>
       <c r="F30">
-        <v>11.21</v>
+        <v>7.99</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1059,19 +1083,19 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>5.81</v>
+        <v>7.24</v>
       </c>
       <c r="C31">
-        <v>6.81</v>
+        <v>7.75</v>
       </c>
       <c r="D31">
-        <v>7.45</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E31">
-        <v>6.41</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F31">
-        <v>9.1</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1079,19 +1103,19 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>4.82</v>
+        <v>11.91</v>
       </c>
       <c r="C32">
-        <v>5.28</v>
+        <v>13.37</v>
       </c>
       <c r="D32">
-        <v>6.36</v>
+        <v>14.79</v>
       </c>
       <c r="E32">
-        <v>5.33</v>
+        <v>12.66</v>
       </c>
       <c r="F32">
-        <v>7.99</v>
+        <v>18.13</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1099,19 +1123,19 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>7.24</v>
+        <v>7.48</v>
       </c>
       <c r="C33">
-        <v>7.75</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="D33">
-        <v>9.699999999999999</v>
+        <v>10.05</v>
       </c>
       <c r="E33">
-        <v>8.300000000000001</v>
+        <v>8.19</v>
       </c>
       <c r="F33">
-        <v>11.67</v>
+        <v>13.67</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1119,19 +1143,19 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>11.91</v>
+        <v>6.2</v>
       </c>
       <c r="C34">
-        <v>13.37</v>
+        <v>7.47</v>
       </c>
       <c r="D34">
-        <v>14.79</v>
+        <v>7.22</v>
       </c>
       <c r="E34">
-        <v>12.66</v>
+        <v>8.44</v>
       </c>
       <c r="F34">
-        <v>18.13</v>
+        <v>7.46</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1139,19 +1163,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>7.48</v>
+        <v>14.46</v>
       </c>
       <c r="C35">
-        <v>8.289999999999999</v>
+        <v>19.08</v>
       </c>
       <c r="D35">
-        <v>10.05</v>
+        <v>15.35</v>
       </c>
       <c r="E35">
-        <v>8.19</v>
+        <v>22.02</v>
       </c>
       <c r="F35">
-        <v>13.67</v>
+        <v>14.57</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1159,19 +1183,19 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>6.2</v>
+        <v>16.54</v>
       </c>
       <c r="C36">
-        <v>7.47</v>
+        <v>19.57</v>
       </c>
       <c r="D36">
-        <v>7.22</v>
+        <v>17.47</v>
       </c>
       <c r="E36">
-        <v>8.44</v>
+        <v>22.07</v>
       </c>
       <c r="F36">
-        <v>7.46</v>
+        <v>19.35</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1179,19 +1203,19 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>14.46</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="C37">
-        <v>19.08</v>
+        <v>10.05</v>
       </c>
       <c r="D37">
-        <v>15.35</v>
+        <v>10.18</v>
       </c>
       <c r="E37">
-        <v>22.02</v>
+        <v>11.64</v>
       </c>
       <c r="F37">
-        <v>14.57</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1199,58 +1223,18 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>16.54</v>
+        <v>13.75</v>
       </c>
       <c r="C38">
-        <v>19.57</v>
+        <v>13.93</v>
       </c>
       <c r="D38">
-        <v>17.47</v>
+        <v>21.37</v>
       </c>
       <c r="E38">
-        <v>22.07</v>
+        <v>17.43</v>
       </c>
       <c r="F38">
-        <v>19.35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39">
-        <v>8.369999999999999</v>
-      </c>
-      <c r="C39">
-        <v>10.05</v>
-      </c>
-      <c r="D39">
-        <v>10.18</v>
-      </c>
-      <c r="E39">
-        <v>11.64</v>
-      </c>
-      <c r="F39">
-        <v>10.51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40">
-        <v>13.75</v>
-      </c>
-      <c r="C40">
-        <v>13.93</v>
-      </c>
-      <c r="D40">
-        <v>21.37</v>
-      </c>
-      <c r="E40">
-        <v>17.43</v>
-      </c>
-      <c r="F40">
         <v>17.39</v>
       </c>
     </row>

</xml_diff>